<commit_message>
Todos os métodos da API implementados
Falta a parte de gerar os avisos e mandar e-mails
</commit_message>
<xml_diff>
--- a/api/bandeco.xlsx
+++ b/api/bandeco.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="19875" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="19875" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Requisições" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <author>Guilherme</author>
   </authors>
   <commentList>
-    <comment ref="H7" authorId="0">
+    <comment ref="G7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -34,7 +34,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="0">
+    <comment ref="K7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0">
+    <comment ref="I8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0">
+    <comment ref="I11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J24" authorId="0">
+    <comment ref="I24" authorId="0">
       <text>
         <r>
           <rPr>
@@ -86,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J28" authorId="0">
+    <comment ref="I28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J35" authorId="0">
+    <comment ref="I35" authorId="0">
       <text>
         <r>
           <rPr>
@@ -112,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H43" authorId="0">
+    <comment ref="G43" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H58" authorId="0">
+    <comment ref="G54" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,6 +137,19 @@
           <t>avisos &amp; 1: semana
 avisos &amp; 2: ruim
 avisos &amp; 4: bom</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G55" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Só pode ser nulo caso não exista ouvinte cadastrado</t>
         </r>
       </text>
     </comment>
@@ -198,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="147">
   <si>
     <t>Título</t>
   </si>
@@ -248,9 +261,6 @@
     <t>boolean</t>
   </si>
   <si>
-    <t>Implementação</t>
-  </si>
-  <si>
     <t>busca</t>
   </si>
   <si>
@@ -497,9 +507,6 @@
     <t>Prato[]</t>
   </si>
   <si>
-    <t>delta</t>
-  </si>
-  <si>
     <t>Mais próximo</t>
   </si>
   <si>
@@ -551,9 +558,6 @@
     <t>Busca por pratos com o nome dado. Retorna uma array ordenando-os pela nota</t>
   </si>
   <si>
-    <t>Retorna informações sobre o cardápio numa data (ou na data mais próxima posterior). Se não houver dados, retorna null. Para facilmente pegar refeições antes ou depois, basta usar o parâmetro delta</t>
-  </si>
-  <si>
     <t>Retorna informações sobre a família e as últimas refeições com essa família. Caso a família não seja encontrada, retorna null</t>
   </si>
   <si>
@@ -590,13 +594,7 @@
     <t>Retorna os últimos avisos disparados (máximo de 10)</t>
   </si>
   <si>
-    <t>temOuvinte</t>
-  </si>
-  <si>
     <t>getOuvinte</t>
-  </si>
-  <si>
-    <t>Verifica se o RA fornecido tem ouvinte registrado a ele</t>
   </si>
   <si>
     <t>Essa aba descreve toda a API baseada em requisições HTTP
@@ -632,18 +630,12 @@
     <t>Remove todas as notificações do usuário. Retorna true em caso de êxito</t>
   </si>
   <si>
-    <t>Atualiza os dados de um ouvinte. Retorna true em caso de êxito. A chave só precisa ser enviada caso o ouvinte já tenha sido registrado</t>
-  </si>
-  <si>
     <t>Indica o tipo de avisos disparados</t>
   </si>
   <si>
     <t>pedirChave</t>
   </si>
   <si>
-    <t>Envia a chave por e-mail</t>
-  </si>
-  <si>
     <t>infoFamilia</t>
   </si>
   <si>
@@ -654,6 +646,15 @@
   </si>
   <si>
     <t>Indica a posição do item (nulo se o objeto não estiver na lista do ranking)</t>
+  </si>
+  <si>
+    <t>Retorna informações sobre o cardápio numa data (ou na data mais próxima posterior). Se não houver dados, retorna null.</t>
+  </si>
+  <si>
+    <t>Envia a chave por e-mail (retorna false caso não precise)</t>
+  </si>
+  <si>
+    <t>Atualiza os dados de um ouvinte. Retorna true em caso de êxito. A chave só precisa ser enviada caso o ouvinte já tenha sido registrado. Valores nulos não serão atualizados</t>
   </si>
 </sst>
 </file>
@@ -711,7 +712,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -834,15 +835,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -893,32 +885,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -926,58 +963,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1293,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z94"/>
+  <dimension ref="A1:Z90"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1305,21 +1297,21 @@
     <col min="2" max="2" width="2.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="2.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="4.7109375" style="2" customWidth="1"/>
-    <col min="15" max="26" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="2" customWidth="1"/>
+    <col min="14" max="25" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="0" style="2" hidden="1"/>
     <col min="27" max="16384" width="9.140625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1333,9 +1325,8 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1348,1028 +1339,915 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="C3" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C3" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="C5" s="25" t="s">
-        <v>133</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C5" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="40" t="s">
+      <c r="D7" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="G7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="L7" s="32" t="s">
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="K7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="40"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="42"/>
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="H8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="33"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K8" s="34"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K9" s="7"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="L10" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C10" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="K10" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="36"/>
-      <c r="H11" s="17" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="25"/>
+      <c r="G11" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="16">
+        <v>20</v>
+      </c>
+      <c r="K11" s="25"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="26"/>
+      <c r="G12" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="17">
-        <v>20</v>
-      </c>
-      <c r="L11" s="36"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="41"/>
-      <c r="H12" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L12" s="41"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="26"/>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="L13" s="22"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K13" s="20"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="C14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="H14" s="17" t="s">
+      <c r="C14" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="25"/>
+      <c r="G15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="25"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="25"/>
+      <c r="G16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="17" t="s">
+      <c r="H16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="L14" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="36"/>
-      <c r="H15" s="17" t="s">
+      <c r="K16" s="25"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="25"/>
+      <c r="G17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="L15" s="36"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="36"/>
-      <c r="H16" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="L16" s="36"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="36"/>
-      <c r="H17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="17" t="s">
+      <c r="H17" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="L17" s="36"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="I17" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="25"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="36"/>
-      <c r="H18" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="17">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="26"/>
+      <c r="G18" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="26"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="K19" s="20"/>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="C20" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="23">
         <v>0</v>
       </c>
-      <c r="L18" s="36"/>
-      <c r="N18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="L19" s="41"/>
-      <c r="N19" s="1"/>
-    </row>
-    <row r="20" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="L20" s="22"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="K20" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="G21" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="13" t="s">
-        <v>129</v>
-      </c>
       <c r="H21" s="12" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="12">
-        <v>0</v>
-      </c>
-      <c r="L21" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K21" s="26"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="L22" s="22"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K22" s="20"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="21"/>
-      <c r="L23" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C23" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="19"/>
+      <c r="K23" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="25"/>
-      <c r="H24" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="21">
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="G24" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="19">
         <v>10</v>
       </c>
-      <c r="L24" s="36"/>
-      <c r="N24" s="1"/>
-    </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K24" s="25"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="25"/>
-      <c r="H25" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="L25" s="41"/>
-      <c r="N25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="G25" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K25" s="26"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="L26" s="22"/>
-      <c r="N26" s="1"/>
-    </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K26" s="20"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="C27" s="42" t="s">
-        <v>148</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="21"/>
-      <c r="L27" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C27" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="19"/>
+      <c r="K27" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="25"/>
-      <c r="H28" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J28" s="21">
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="32"/>
+      <c r="G28" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28" s="19">
         <v>10</v>
       </c>
-      <c r="L28" s="36"/>
-      <c r="N28" s="1"/>
-    </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K28" s="25"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="25"/>
-      <c r="H29" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I29" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="L29" s="41"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="30"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="G29" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="K29" s="26"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="L30" s="22"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K30" s="20"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="C31" s="42" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="25" t="s">
-        <v>120</v>
+      <c r="C31" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31" s="10"/>
-      <c r="L31" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="N31" s="1"/>
-    </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="I31" s="10"/>
+      <c r="K31" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="25"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="32"/>
+      <c r="G32" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="H32" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J32" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="L32" s="41"/>
-      <c r="N32" s="1"/>
-    </row>
-    <row r="33" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K32" s="26"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="C33" s="6"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="L33" s="22"/>
-      <c r="N33" s="1"/>
-    </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K33" s="20"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="C34" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="35" t="s">
+      <c r="C34" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="16">
+        <v>0</v>
+      </c>
+      <c r="K34" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="25"/>
+      <c r="G35" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="H34" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J34" s="17">
-        <v>0</v>
-      </c>
-      <c r="L34" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="N34" s="1"/>
-    </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="36"/>
-      <c r="H35" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J35" s="17">
+      <c r="H35" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="16">
         <v>10</v>
       </c>
-      <c r="L35" s="36"/>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K35" s="25"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="41"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="26"/>
+      <c r="G36" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="H36" s="8" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L36" s="41"/>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K36" s="26"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="6"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="L37" s="22"/>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K37" s="20"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="35" t="s">
-        <v>112</v>
+      <c r="C38" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K38" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="L38" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="41"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="26"/>
+      <c r="G39" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="H39" s="8" t="s">
-        <v>95</v>
+        <v>31</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L39" s="41"/>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K39" s="26"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="L40" s="22"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K40" s="20"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="C41" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="29"/>
-      <c r="F41" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="I41" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J41" s="17"/>
-      <c r="L41" s="35" t="s">
+      <c r="C41" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I41" s="16"/>
+      <c r="K41" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="36"/>
-      <c r="H42" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I42" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J42" s="17"/>
-      <c r="L42" s="36"/>
-      <c r="N42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="25"/>
+      <c r="G42" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="16"/>
+      <c r="K42" s="25"/>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="41"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="26"/>
+      <c r="G43" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="H43" s="8" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L43" s="41"/>
-      <c r="N43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K43" s="26"/>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="C44" s="6"/>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="L44" s="22"/>
-      <c r="N44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="20"/>
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="C45" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D45" s="18" t="s">
+      <c r="C45" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J45" s="17"/>
-      <c r="L45" s="16" t="s">
+      <c r="E45" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" s="8"/>
+      <c r="K45" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="C46" s="6"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="L46" s="22"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="20"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="C47" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="16" t="s">
-        <v>146</v>
+      <c r="C47" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J47" s="8"/>
-      <c r="L47" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="I47" s="8"/>
+      <c r="K47" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="C48" s="6"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
-      <c r="J48" s="7"/>
-      <c r="L48" s="22"/>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="K48" s="20"/>
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="C49" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="D49" s="37" t="s">
+      <c r="C49" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="I49" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J49" s="8"/>
-      <c r="L49" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="N49" s="1"/>
-    </row>
-    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="E49" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="G49" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="K49" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="36"/>
-      <c r="H50" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I50" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J50" s="8"/>
-      <c r="L50" s="36"/>
-      <c r="N50" s="1"/>
-    </row>
-    <row r="51" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="6"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="K50" s="20"/>
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="7"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="L51" s="22"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C51" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51" s="8"/>
+      <c r="K51" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="C52" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="29" t="s">
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="32"/>
+      <c r="G52" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="K52" s="25"/>
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="32"/>
+      <c r="G53" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K53" s="25"/>
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="32"/>
+      <c r="G54" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E52" s="29"/>
-      <c r="F52" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I52" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J52" s="17"/>
-      <c r="L52" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="41"/>
-      <c r="H53" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="I53" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J53" s="8"/>
-      <c r="L53" s="41"/>
-      <c r="N53" s="1"/>
-    </row>
-    <row r="54" spans="1:14" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="L54" s="22"/>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="H54" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="K54" s="25"/>
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="C55" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="E55" s="26"/>
-      <c r="F55" s="25" t="s">
-        <v>143</v>
+      <c r="C55" s="36"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="32"/>
+      <c r="G55" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J55" s="8"/>
-      <c r="L55" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="N55" s="1"/>
-    </row>
-    <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K55" s="26"/>
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="25"/>
-      <c r="H56" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J56" s="11"/>
-      <c r="L56" s="36"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="25"/>
-      <c r="H57" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I57" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J57" s="8"/>
-      <c r="L57" s="36"/>
-      <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="25"/>
-      <c r="H58" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="I58" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J58" s="17"/>
-      <c r="L58" s="36"/>
-      <c r="N58" s="1"/>
-    </row>
-    <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="25"/>
-      <c r="H59" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I59" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J59" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L59" s="41"/>
-      <c r="N59" s="1"/>
-    </row>
-    <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:13" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2396,75 +2274,55 @@
     <row r="88" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="89" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="90" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="L55:L59"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="L41:L43"/>
-    <mergeCell ref="L31:L32"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="L27:L29"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="C14:C19"/>
-    <mergeCell ref="D14:D19"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="F14:F19"/>
-    <mergeCell ref="L14:L19"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D55:D59"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F23:F25"/>
+  <mergeCells count="47">
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="E38:E39"/>
     <mergeCell ref="D38:D39"/>
-    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="C51:C55"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C3:L3"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="E55:E59"/>
-    <mergeCell ref="F55:F59"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="K14:K18"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="K41:K43"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="K51:K55"/>
+    <mergeCell ref="D51:D55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2476,8 +2334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2517,7 +2375,7 @@
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="C3" s="43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="43"/>
       <c r="E3" s="43"/>
@@ -2531,7 +2389,7 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" s="44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
@@ -2544,16 +2402,16 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="1"/>
@@ -2564,73 +2422,73 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>28</v>
-      </c>
       <c r="E9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" s="30"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="30"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" s="30"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="C13" s="31"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>37</v>
+      <c r="F13" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="1"/>
@@ -2649,59 +2507,59 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="C17" s="30"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="C18" s="31"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -2719,101 +2577,101 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="C20" s="29" t="s">
-        <v>48</v>
+      <c r="C20" s="27" t="s">
+        <v>47</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="30"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="C22" s="30"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="30"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>59</v>
+      <c r="C24" s="29"/>
+      <c r="D24" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="C25" s="30"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>60</v>
+        <v>43</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="C26" s="31"/>
+      <c r="C26" s="28"/>
       <c r="D26" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>61</v>
+        <v>31</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>60</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -2831,31 +2689,31 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>65</v>
+      <c r="E28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>150</v>
+      <c r="C29" s="28"/>
+      <c r="D29" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -2873,59 +2731,59 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="C31" s="29" t="s">
-        <v>123</v>
+      <c r="C31" s="27" t="s">
+        <v>120</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="21" t="s">
-        <v>126</v>
+      <c r="C32" s="29"/>
+      <c r="D32" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="21" t="s">
-        <v>127</v>
+      <c r="C33" s="29"/>
+      <c r="D33" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="C34" s="31"/>
+      <c r="C34" s="28"/>
       <c r="D34" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -2943,199 +2801,199 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="C36" s="29" t="s">
-        <v>66</v>
+      <c r="C36" s="27" t="s">
+        <v>65</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="C37" s="30"/>
+      <c r="C37" s="29"/>
       <c r="D37" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="30"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="C39" s="30"/>
+      <c r="C39" s="29"/>
       <c r="D39" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="C40" s="30"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="C41" s="30"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="C42" s="30"/>
+      <c r="C42" s="29"/>
       <c r="D42" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F43" s="21" t="s">
-        <v>82</v>
+      <c r="C43" s="29"/>
+      <c r="D43" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="21" t="s">
-        <v>85</v>
+      <c r="C44" s="29"/>
+      <c r="D44" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F45" s="21" t="s">
-        <v>86</v>
+      <c r="C45" s="29"/>
+      <c r="D45" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="17" t="s">
+      <c r="C46" s="29"/>
+      <c r="D46" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="21" t="s">
-        <v>87</v>
+      <c r="F46" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="21" t="s">
-        <v>88</v>
+      <c r="C47" s="29"/>
+      <c r="D47" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F48" s="21" t="s">
-        <v>90</v>
+      <c r="C48" s="29"/>
+      <c r="D48" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="C49" s="31"/>
+      <c r="C49" s="28"/>
       <c r="D49" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H49" s="1"/>
     </row>
@@ -3153,59 +3011,59 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="C51" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="21" t="s">
-        <v>138</v>
+      <c r="C51" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>133</v>
       </c>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E52" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" s="21" t="s">
-        <v>139</v>
+      <c r="C52" s="29"/>
+      <c r="D52" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>134</v>
       </c>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E53" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" s="21" t="s">
-        <v>140</v>
+      <c r="C53" s="29"/>
+      <c r="D53" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>144</v>
+      <c r="C54" s="28"/>
+      <c r="D54" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>138</v>
       </c>
       <c r="H54" s="1"/>
     </row>

</xml_diff>

<commit_message>
Interface para configurar os avisos pelo WebApp
</commit_message>
<xml_diff>
--- a/api/bandeco.xlsx
+++ b/api/bandeco.xlsx
@@ -895,58 +895,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1319,17 +1319,17 @@
     </row>
     <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1338,17 +1338,17 @@
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1357,30 +1357,30 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="K7" s="33" t="s">
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="K7" s="35" t="s">
         <v>2</v>
       </c>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="39"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="30"/>
       <c r="G8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1390,7 +1390,7 @@
       <c r="I8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="34"/>
+      <c r="K8" s="36"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -1406,10 +1406,10 @@
     </row>
     <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="38" t="s">
         <v>80</v>
       </c>
       <c r="E10" s="23" t="s">
@@ -1429,9 +1429,9 @@
     </row>
     <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="24"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="31"/>
       <c r="G11" s="14" t="s">
         <v>84</v>
       </c>
@@ -1441,14 +1441,14 @@
       <c r="I11" s="14">
         <v>20</v>
       </c>
-      <c r="K11" s="24"/>
+      <c r="K11" s="31"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="25"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="24"/>
       <c r="G12" s="6" t="s">
         <v>83</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="I12" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K12" s="25"/>
+      <c r="K12" s="24"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1474,10 +1474,10 @@
     </row>
     <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="38" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="23" t="s">
@@ -1499,9 +1499,9 @@
     </row>
     <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="24"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="31"/>
       <c r="G15" s="14" t="s">
         <v>22</v>
       </c>
@@ -1511,14 +1511,14 @@
       <c r="I15" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="K15" s="24"/>
+      <c r="K15" s="31"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="24"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="31"/>
       <c r="G16" s="14" t="s">
         <v>21</v>
       </c>
@@ -1528,14 +1528,14 @@
       <c r="I16" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="K16" s="24"/>
+      <c r="K16" s="31"/>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="24"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="31"/>
       <c r="G17" s="14" t="s">
         <v>23</v>
       </c>
@@ -1545,14 +1545,14 @@
       <c r="I17" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="K17" s="24"/>
+      <c r="K17" s="31"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="25"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="24"/>
       <c r="G18" s="10" t="s">
         <v>83</v>
       </c>
@@ -1562,7 +1562,7 @@
       <c r="I18" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="K18" s="25"/>
+      <c r="K18" s="24"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,10 +1578,10 @@
     </row>
     <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="38" t="s">
         <v>80</v>
       </c>
       <c r="E20" s="23" t="s">
@@ -1603,9 +1603,9 @@
     </row>
     <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="25"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="24"/>
       <c r="G21" s="10" t="s">
         <v>83</v>
       </c>
@@ -1615,7 +1615,7 @@
       <c r="I21" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="K21" s="25"/>
+      <c r="K21" s="24"/>
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1631,13 +1631,13 @@
     </row>
     <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="27" t="s">
         <v>104</v>
       </c>
       <c r="G23" s="14" t="s">
@@ -1654,9 +1654,9 @@
     </row>
     <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="27"/>
       <c r="G24" s="14" t="s">
         <v>94</v>
       </c>
@@ -1666,14 +1666,14 @@
       <c r="I24" s="22">
         <v>10</v>
       </c>
-      <c r="K24" s="24"/>
+      <c r="K24" s="31"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="27"/>
       <c r="G25" s="14" t="s">
         <v>83</v>
       </c>
@@ -1683,7 +1683,7 @@
       <c r="I25" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K25" s="25"/>
+      <c r="K25" s="24"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1699,13 +1699,13 @@
     </row>
     <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="27" t="s">
         <v>105</v>
       </c>
       <c r="G27" s="14" t="s">
@@ -1722,9 +1722,9 @@
     </row>
     <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="27"/>
       <c r="G28" s="14" t="s">
         <v>94</v>
       </c>
@@ -1734,14 +1734,14 @@
       <c r="I28" s="22">
         <v>10</v>
       </c>
-      <c r="K28" s="24"/>
+      <c r="K28" s="31"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="27"/>
       <c r="G29" s="14" t="s">
         <v>83</v>
       </c>
@@ -1751,7 +1751,7 @@
       <c r="I29" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="K29" s="25"/>
+      <c r="K29" s="24"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1767,13 +1767,13 @@
     </row>
     <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="27" t="s">
         <v>106</v>
       </c>
       <c r="G31" s="6" t="s">
@@ -1790,9 +1790,9 @@
     </row>
     <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="27"/>
       <c r="G32" s="6" t="s">
         <v>83</v>
       </c>
@@ -1802,7 +1802,7 @@
       <c r="I32" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="K32" s="25"/>
+      <c r="K32" s="24"/>
       <c r="M32" s="1"/>
     </row>
     <row r="33" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1818,10 +1818,10 @@
     </row>
     <row r="34" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="27" t="s">
+      <c r="D34" s="38" t="s">
         <v>80</v>
       </c>
       <c r="E34" s="23" t="s">
@@ -1843,9 +1843,9 @@
     </row>
     <row r="35" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="24"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="31"/>
       <c r="G35" s="14" t="s">
         <v>97</v>
       </c>
@@ -1855,14 +1855,14 @@
       <c r="I35" s="14">
         <v>10</v>
       </c>
-      <c r="K35" s="24"/>
+      <c r="K35" s="31"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="25"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="24"/>
       <c r="G36" s="6" t="s">
         <v>83</v>
       </c>
@@ -1872,7 +1872,7 @@
       <c r="I36" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K36" s="25"/>
+      <c r="K36" s="24"/>
       <c r="M36" s="1"/>
     </row>
     <row r="37" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1888,10 +1888,10 @@
     </row>
     <row r="38" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="32" t="s">
         <v>80</v>
       </c>
       <c r="E38" s="23" t="s">
@@ -1913,9 +1913,9 @@
     </row>
     <row r="39" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="25"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="24"/>
       <c r="G39" s="6" t="s">
         <v>83</v>
       </c>
@@ -1925,7 +1925,7 @@
       <c r="I39" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K39" s="25"/>
+      <c r="K39" s="24"/>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -1941,10 +1941,10 @@
     </row>
     <row r="41" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="38" t="s">
         <v>81</v>
       </c>
       <c r="E41" s="23" t="s">
@@ -1964,9 +1964,9 @@
     </row>
     <row r="42" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="24"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="31"/>
       <c r="G42" s="14" t="s">
         <v>83</v>
       </c>
@@ -1974,14 +1974,14 @@
         <v>24</v>
       </c>
       <c r="I42" s="14"/>
-      <c r="K42" s="24"/>
+      <c r="K42" s="31"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="25"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="24"/>
       <c r="G43" s="6" t="s">
         <v>101</v>
       </c>
@@ -1991,7 +1991,7 @@
       <c r="I43" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K43" s="25"/>
+      <c r="K43" s="24"/>
       <c r="M43" s="1"/>
     </row>
     <row r="44" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
       <c r="K46" s="18"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="C47" s="21" t="s">
         <v>116</v>
@@ -2109,13 +2109,13 @@
     </row>
     <row r="51" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="C51" s="26" t="s">
+      <c r="C51" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="26" t="s">
+      <c r="D51" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="E51" s="32" t="s">
+      <c r="E51" s="27" t="s">
         <v>135</v>
       </c>
       <c r="G51" s="6" t="s">
@@ -2132,9 +2132,9 @@
     </row>
     <row r="52" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="32"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="27"/>
       <c r="G52" s="9" t="s">
         <v>121</v>
       </c>
@@ -2144,14 +2144,14 @@
       <c r="I52" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="K52" s="24"/>
+      <c r="K52" s="31"/>
       <c r="M52" s="1"/>
     </row>
     <row r="53" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="32"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="27"/>
       <c r="G53" s="6" t="s">
         <v>32</v>
       </c>
@@ -2161,14 +2161,14 @@
       <c r="I53" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K53" s="24"/>
+      <c r="K53" s="31"/>
       <c r="M53" s="1"/>
     </row>
     <row r="54" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="32"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="27"/>
       <c r="G54" s="14" t="s">
         <v>82</v>
       </c>
@@ -2178,14 +2178,14 @@
       <c r="I54" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="K54" s="24"/>
+      <c r="K54" s="31"/>
       <c r="M54" s="1"/>
     </row>
     <row r="55" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="32"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="27"/>
       <c r="G55" s="6" t="s">
         <v>119</v>
       </c>
@@ -2195,7 +2195,7 @@
       <c r="I55" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="K55" s="25"/>
+      <c r="K55" s="24"/>
       <c r="M55" s="1"/>
     </row>
     <row r="56" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -2252,6 +2252,37 @@
     <row r="90" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="K51:K55"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="K23:K25"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="K41:K43"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="K27:K29"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="K14:K18"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="K20:K21"/>
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="C5:K5"/>
@@ -2268,37 +2299,6 @@
     <mergeCell ref="C34:C36"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="D14:D18"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="K14:K18"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="K27:K29"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="K41:K43"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="K51:K55"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="K23:K25"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="K38:K39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2310,7 +2310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="38" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -2414,7 +2414,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" s="28"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="10" t="s">
         <v>22</v>
       </c>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="C11" s="28"/>
+      <c r="C11" s="39"/>
       <c r="D11" s="10" t="s">
         <v>21</v>
       </c>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" s="28"/>
+      <c r="C12" s="39"/>
       <c r="D12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="C13" s="29"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="10" t="s">
         <v>23</v>
       </c>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="38" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -2499,7 +2499,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="C16" s="28"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="10" t="s">
         <v>32</v>
       </c>
@@ -2513,7 +2513,7 @@
     </row>
     <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="C17" s="28"/>
+      <c r="C17" s="39"/>
       <c r="D17" s="10" t="s">
         <v>43</v>
       </c>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="C18" s="29"/>
+      <c r="C18" s="40"/>
       <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="38" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="10" t="s">
@@ -2569,7 +2569,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="C21" s="28"/>
+      <c r="C21" s="39"/>
       <c r="D21" s="10" t="s">
         <v>44</v>
       </c>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="C22" s="28"/>
+      <c r="C22" s="39"/>
       <c r="D22" s="10" t="s">
         <v>32</v>
       </c>
@@ -2597,7 +2597,7 @@
     </row>
     <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="C23" s="28"/>
+      <c r="C23" s="39"/>
       <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="C24" s="28"/>
+      <c r="C24" s="39"/>
       <c r="D24" s="14" t="s">
         <v>33</v>
       </c>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="C25" s="28"/>
+      <c r="C25" s="39"/>
       <c r="D25" s="10" t="s">
         <v>45</v>
       </c>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="26" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="C26" s="29"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="10" t="s">
         <v>46</v>
       </c>
@@ -2665,7 +2665,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="38" t="s">
         <v>54</v>
       </c>
       <c r="D28" s="14" t="s">
@@ -2681,7 +2681,7 @@
     </row>
     <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="C29" s="29"/>
+      <c r="C29" s="40"/>
       <c r="D29" s="14" t="s">
         <v>56</v>
       </c>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="38" t="s">
         <v>109</v>
       </c>
       <c r="D31" s="10" t="s">
@@ -2723,7 +2723,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="C32" s="28"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="14" t="s">
         <v>110</v>
       </c>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="C33" s="28"/>
+      <c r="C33" s="39"/>
       <c r="D33" s="14" t="s">
         <v>92</v>
       </c>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="C34" s="29"/>
+      <c r="C34" s="40"/>
       <c r="D34" s="10" t="s">
         <v>59</v>
       </c>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="38" t="s">
         <v>58</v>
       </c>
       <c r="D36" s="10" t="s">
@@ -2793,7 +2793,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="C37" s="28"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="10" t="s">
         <v>59</v>
       </c>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="28"/>
+      <c r="C38" s="39"/>
       <c r="D38" s="10" t="s">
         <v>60</v>
       </c>
@@ -2821,7 +2821,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="C39" s="28"/>
+      <c r="C39" s="39"/>
       <c r="D39" s="10" t="s">
         <v>61</v>
       </c>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="C40" s="28"/>
+      <c r="C40" s="39"/>
       <c r="D40" s="10" t="s">
         <v>62</v>
       </c>
@@ -2849,7 +2849,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="C41" s="28"/>
+      <c r="C41" s="39"/>
       <c r="D41" s="10" t="s">
         <v>63</v>
       </c>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="C42" s="28"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="10" t="s">
         <v>64</v>
       </c>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="C43" s="28"/>
+      <c r="C43" s="39"/>
       <c r="D43" s="14" t="s">
         <v>65</v>
       </c>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="C44" s="28"/>
+      <c r="C44" s="39"/>
       <c r="D44" s="14" t="s">
         <v>43</v>
       </c>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="C45" s="28"/>
+      <c r="C45" s="39"/>
       <c r="D45" s="14" t="s">
         <v>45</v>
       </c>
@@ -2919,7 +2919,7 @@
     </row>
     <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="C46" s="28"/>
+      <c r="C46" s="39"/>
       <c r="D46" s="14" t="s">
         <v>66</v>
       </c>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="C47" s="28"/>
+      <c r="C47" s="39"/>
       <c r="D47" s="14" t="s">
         <v>33</v>
       </c>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="38" t="s">
         <v>120</v>
       </c>
       <c r="D49" s="14" t="s">
@@ -2975,7 +2975,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="C50" s="28"/>
+      <c r="C50" s="39"/>
       <c r="D50" s="14" t="s">
         <v>121</v>
       </c>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="C51" s="28"/>
+      <c r="C51" s="39"/>
       <c r="D51" s="14" t="s">
         <v>32</v>
       </c>
@@ -3003,7 +3003,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="C52" s="29"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="14" t="s">
         <v>82</v>
       </c>

</xml_diff>